<commit_message>
Local Database Setup for TestReply Module Done
</commit_message>
<xml_diff>
--- a/my_project/db/questionDetails.xlsx
+++ b/my_project/db/questionDetails.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,23 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>agnihotriaman@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>124ef1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{1: 'e_que_1', 2: 'm_stck_8', 3: 'm_ll_7', 4: 'm_que_7', 5: 'm_str_2', 6: 'e_que_3', 7: 'm_ll_9', 8: 'e_que_7'}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>